<commit_message>
Mockup more or less done
</commit_message>
<xml_diff>
--- a/frontend-app/frontend-project/public/Site_diary_day.xlsx
+++ b/frontend-app/frontend-project/public/Site_diary_day.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\AI_demo_project\10.04.2024 Actual project React + Backend\frontend-app\frontend-project\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A3E2DA35-1FF1-4233-A78B-44D35972F911}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFDF8268-F30E-434A-AB86-4AC9ECBCC4F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{52DB515E-9390-457C-ABD7-D29C65D8E7A7}"/>
+    <workbookView xWindow="14295" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{52DB515E-9390-457C-ABD7-D29C65D8E7A7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,6 +35,65 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="18">
+  <si>
+    <t>Works</t>
+  </si>
+  <si>
+    <t>Location</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>Fondations</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Finishin works </t>
+  </si>
+  <si>
+    <t>Workers</t>
+  </si>
+  <si>
+    <t>Hours</t>
+  </si>
+  <si>
+    <t>Project amounts</t>
+  </si>
+  <si>
+    <t>500m2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Completed </t>
+  </si>
+  <si>
+    <t>First floor</t>
+  </si>
+  <si>
+    <t>Assembly</t>
+  </si>
+  <si>
+    <t>100m2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Concreeting </t>
+  </si>
+  <si>
+    <t>80m3</t>
+  </si>
+  <si>
+    <t>20m3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Photos : </t>
+  </si>
+  <si>
+    <t>Delivered materials</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
@@ -55,7 +114,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -63,12 +122,110 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -403,12 +560,197 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A429FC50-29C9-4AD2-A5C8-92A95CAE352C}">
-  <dimension ref="A1"/>
+  <dimension ref="A6:G21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7:G21"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="18.7109375" customWidth="1"/>
+    <col min="2" max="3" width="14.42578125" customWidth="1"/>
+    <col min="6" max="6" width="17.28515625" customWidth="1"/>
+    <col min="7" max="7" width="12.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="6" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="4"/>
+      <c r="B8" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D8" s="5">
+        <v>3</v>
+      </c>
+      <c r="E8" s="5">
+        <f>D8*4</f>
+        <v>12</v>
+      </c>
+      <c r="F8" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="G8" s="7" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="4"/>
+      <c r="B9" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D9" s="5">
+        <v>2</v>
+      </c>
+      <c r="E9" s="5">
+        <v>15</v>
+      </c>
+      <c r="F9" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="G9" s="7" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="8"/>
+      <c r="B10" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="C10" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="D10" s="9">
+        <v>4</v>
+      </c>
+      <c r="E10" s="9">
+        <f>4*9</f>
+        <v>36</v>
+      </c>
+      <c r="F10" s="9">
+        <v>60</v>
+      </c>
+      <c r="G10" s="10">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B12" s="2"/>
+      <c r="C12" s="2"/>
+      <c r="D12" s="2"/>
+      <c r="E12" s="2"/>
+      <c r="F12" s="2"/>
+      <c r="G12" s="3"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="4"/>
+      <c r="B13" s="5"/>
+      <c r="C13" s="5"/>
+      <c r="D13" s="5"/>
+      <c r="E13" s="5"/>
+      <c r="F13" s="5"/>
+      <c r="G13" s="11"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="4"/>
+      <c r="B14" s="5"/>
+      <c r="C14" s="5"/>
+      <c r="D14" s="5"/>
+      <c r="E14" s="5"/>
+      <c r="F14" s="5"/>
+      <c r="G14" s="11"/>
+    </row>
+    <row r="15" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="8"/>
+      <c r="B15" s="9"/>
+      <c r="C15" s="9"/>
+      <c r="D15" s="9"/>
+      <c r="E15" s="9"/>
+      <c r="F15" s="9"/>
+      <c r="G15" s="12"/>
+    </row>
+    <row r="16" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B17" s="2"/>
+      <c r="C17" s="2"/>
+      <c r="D17" s="2"/>
+      <c r="E17" s="2"/>
+      <c r="F17" s="2"/>
+      <c r="G17" s="3"/>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" s="4"/>
+      <c r="B18" s="5"/>
+      <c r="C18" s="5"/>
+      <c r="D18" s="5"/>
+      <c r="E18" s="5"/>
+      <c r="F18" s="5"/>
+      <c r="G18" s="11"/>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" s="4"/>
+      <c r="B19" s="5"/>
+      <c r="C19" s="5"/>
+      <c r="D19" s="5"/>
+      <c r="E19" s="5"/>
+      <c r="F19" s="5"/>
+      <c r="G19" s="11"/>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" s="4"/>
+      <c r="B20" s="5"/>
+      <c r="C20" s="5"/>
+      <c r="D20" s="5"/>
+      <c r="E20" s="5"/>
+      <c r="F20" s="5"/>
+      <c r="G20" s="11"/>
+    </row>
+    <row r="21" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="8"/>
+      <c r="B21" s="9"/>
+      <c r="C21" s="9"/>
+      <c r="D21" s="9"/>
+      <c r="E21" s="9"/>
+      <c r="F21" s="9"/>
+      <c r="G21" s="12"/>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>